<commit_message>
Update MATLAB source code
</commit_message>
<xml_diff>
--- a/CryoGrid/CryoGridCommunity_results/CG_single/CG_single.xlsx
+++ b/CryoGrid/CryoGridCommunity_results/CG_single/CG_single.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="346039" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="353583" uniqueCount="221">
   <si>
     <t>-------------------</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>FORCING_data_elev_3149_slope_0_aspect_-1_massif_15_dates_01Aug1958_01Aug2024_MON1.mat</t>
+  </si>
+  <si>
+    <t>/Users/maximefadel/Documents/Stage_Edytem/CryoGrid_Optimization_Automatization/forcing/Forcing_Data/</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1147,7 @@
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.5703125" customWidth="true"/>
-    <col min="2" max="2" width="106.42578125" customWidth="true"/>
+    <col min="2" max="2" width="99.7109375" customWidth="true"/>
     <col min="3" max="3" width="35.5703125" bestFit="true" customWidth="true"/>
     <col min="4" max="4" width="138.28515625" customWidth="true"/>
     <col min="5" max="5" width="22.28515625" customWidth="true"/>
@@ -1342,7 +1345,7 @@
         <v>161</v>
       </c>
       <c r="B13" s="9">
-        <v>44.078111999999898</v>
+        <v>45.299999999999997</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>163</v>
@@ -1368,7 +1371,7 @@
         <v>162</v>
       </c>
       <c r="B14" s="9">
-        <v>7.4269150000000002</v>
+        <v>6.5</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
@@ -1384,7 +1387,7 @@
         <v>163</v>
       </c>
       <c r="B15" s="9">
-        <v>2929.6790999999998</v>
+        <v>3149</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>186</v>
@@ -1402,7 +1405,7 @@
         <v>181</v>
       </c>
       <c r="B16" s="12">
-        <v>35.432518005371087</v>
+        <v>24.259347915649411</v>
       </c>
       <c r="C16" s="0"/>
       <c r="D16" s="0"/>
@@ -1418,7 +1421,7 @@
         <v>182</v>
       </c>
       <c r="B17" s="12">
-        <v>229.63006591796881</v>
+        <v>59.289894104003913</v>
       </c>
       <c r="C17" s="0"/>
       <c r="D17" s="0"/>
@@ -1434,7 +1437,7 @@
         <v>194</v>
       </c>
       <c r="B18" s="18">
-        <v>0.90739944780175486</v>
+        <v>0.95584751093937359</v>
       </c>
       <c r="C18" s="0"/>
       <c r="D18" s="0"/>
@@ -1938,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C50" s="0"/>
       <c r="D50" s="0"/>
@@ -1954,7 +1957,7 @@
         <v>34</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="C51" s="0"/>
       <c r="D51" s="0"/>
@@ -1973,13 +1976,13 @@
         <v>22</v>
       </c>
       <c r="C52" s="9">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D52" s="9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E52" s="9">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>25</v>
@@ -2310,7 +2313,7 @@
         <v>48</v>
       </c>
       <c r="B72" s="0">
-        <v>2931.6790999999998</v>
+        <v>3151</v>
       </c>
       <c r="C72" s="0"/>
       <c r="D72" s="16" t="s">
@@ -2328,7 +2331,7 @@
         <v>50</v>
       </c>
       <c r="B73" s="0">
-        <v>2924.6790999999998</v>
+        <v>3144</v>
       </c>
       <c r="C73" s="0"/>
       <c r="D73" s="16" t="s">
@@ -2400,7 +2403,7 @@
         <v>58</v>
       </c>
       <c r="B77" s="0">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C77" s="0"/>
       <c r="D77" s="16" t="s">
@@ -3237,7 +3240,7 @@
         <v>0</v>
       </c>
       <c r="C127" s="9">
-        <v>0</v>
+        <v>0.13848281731183243</v>
       </c>
       <c r="D127" s="0"/>
       <c r="E127" s="0"/>
@@ -3253,7 +3256,7 @@
         <v>1.5</v>
       </c>
       <c r="C128" s="9">
-        <v>0</v>
+        <v>0.13848281731183243</v>
       </c>
       <c r="D128" s="0"/>
       <c r="E128" s="0"/>
@@ -3269,7 +3272,7 @@
         <v>10</v>
       </c>
       <c r="C129" s="9">
-        <v>0</v>
+        <v>0.13848281731183243</v>
       </c>
       <c r="D129" s="0"/>
       <c r="E129" s="0"/>
@@ -3285,7 +3288,7 @@
         <v>5000</v>
       </c>
       <c r="C130" s="9">
-        <v>0</v>
+        <v>0.13848281731183243</v>
       </c>
       <c r="D130" s="0"/>
       <c r="E130" s="0"/>

</xml_diff>